<commit_message>
GeneratorProperty improvements. User import and delete
</commit_message>
<xml_diff>
--- a/app/public/templates/user_import_template.xlsx
+++ b/app/public/templates/user_import_template.xlsx
@@ -32,12 +32,19 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve">INSTRUCTIONS:
-1. Fill in the required fields: email, name, password
-2. Roles are optional - use comma-separated values (e.g., instructor,admin)
-3. Delete the example row (row 2) before uploading
-4. Maximum file size: 5MB
-5. All imported users will be verified automatically</t>
+          <t xml:space="preserve">USER IMPORT TEMPLATE
+Required fields:
+• email - Must be unique and valid
+• name - Full name (2-255 chars)
+• password - Minimum 6 characters
+Optional fields:
+• roles - Comma-separated (e.g., instructor,admin)
+• openai_api_key - User's OpenAI API key
+Notes:
+• Row 2 is an example - you can keep it or delete it
+• Empty rows (no email) are ignored
+• All imported users are verified
+• Max file size: 5MB</t>
         </r>
       </text>
     </comment>
@@ -46,21 +53,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
-  <si>
-    <t>Email (Required)</t>
-  </si>
-  <si>
-    <t>Name (Required)</t>
-  </si>
-  <si>
-    <t>Password (Required)</t>
-  </si>
-  <si>
-    <t>Roles (Optional)</t>
-  </si>
-  <si>
-    <t>OpenAI API Key (Optional)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>openai_api_key</t>
   </si>
   <si>
     <t>john.doe@example.com</t>
@@ -73,39 +80,6 @@
   </si>
   <si>
     <t>instructor</t>
-  </si>
-  <si>
-    <t>Instructions:</t>
-  </si>
-  <si>
-    <t>• Email: Must be unique and valid email format</t>
-  </si>
-  <si>
-    <t>• Name: Full name of the user (2-255 characters)</t>
-  </si>
-  <si>
-    <t>• Password: Minimum 6 characters</t>
-  </si>
-  <si>
-    <t>• Roles: Optional, comma-separated (e.g., "instructor,admin")</t>
-  </si>
-  <si>
-    <t>• OpenAI API Key: Optional, user's OpenAI API key</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>• All imported users will be set as verified</t>
-  </si>
-  <si>
-    <t>• Users must accept terms on first login</t>
-  </si>
-  <si>
-    <t>• Delete row 2 (example) before uploading</t>
-  </si>
-  <si>
-    <t>• Maximum 1000 users per import recommended</t>
   </si>
 </sst>
 </file>
@@ -113,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -139,24 +113,6 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF6B7280"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -192,14 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +453,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -546,78 +500,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>